<commit_message>
added and removed sections from table that didnt have enough data to support it
</commit_message>
<xml_diff>
--- a/data/data_dictionary_current.xlsx
+++ b/data/data_dictionary_current.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gpain/Documents/Work_Dashboards/Oklahoma/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C90DFD-5710-244F-A2FD-866C0D0F535E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0EB8D5B-67AE-F54B-A749-969928CD7971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30240" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="1" r:id="rId1"/>
@@ -2089,8 +2089,8 @@
   </sheetPr>
   <dimension ref="A1:K123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="C55" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="J81" sqref="J81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2850,7 +2850,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K23" s="3" t="s">
         <v>53</v>
@@ -4578,7 +4578,7 @@
         <v>0</v>
       </c>
       <c r="J77" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K77" s="3" t="s">
         <v>53</v>
@@ -4654,7 +4654,7 @@
         <v>0</v>
       </c>
       <c r="J80" s="5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K80" s="3" t="s">
         <v>53</v>
@@ -4686,7 +4686,7 @@
         <v>0</v>
       </c>
       <c r="J81" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K81" s="3" t="s">
         <v>53</v>
@@ -5903,7 +5903,7 @@
   </sheetPr>
   <dimension ref="A1:N94"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A38" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>